<commit_message>
add see doc and upload
</commit_message>
<xml_diff>
--- a/UML.xlsx
+++ b/UML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novem\thesis-demo\thesis-demo-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6505B2E7-58DB-4FA6-9155-FD07BC9006E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231EB36-8DFE-4F36-A649-4D3D80F01329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5B04DCB9-39D0-4E64-9D51-FA2307D7CDD8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="35">
   <si>
     <t>No.</t>
   </si>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEEF4B8-D47D-4B74-827B-029011FA4996}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H1" sqref="H1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +510,7 @@
     <col min="5" max="5" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,8 +526,20 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -543,8 +555,20 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -560,8 +584,20 @@
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -577,8 +613,20 @@
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -594,8 +642,20 @@
       <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H5" s="3">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -611,8 +671,20 @@
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H6" s="3">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -628,8 +700,20 @@
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H7" s="3">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -645,8 +729,20 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H8" s="3">
+        <v>7</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -662,8 +758,20 @@
       <c r="E9" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H9" s="3">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -679,8 +787,20 @@
       <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H10" s="3">
+        <v>9</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -696,8 +816,20 @@
       <c r="E11" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H11" s="3">
+        <v>10</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -713,8 +845,20 @@
       <c r="E12" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H12" s="3">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -730,8 +874,20 @@
       <c r="E13" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H13" s="3">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -747,8 +903,20 @@
       <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H14" s="3">
+        <v>13</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -762,6 +930,18 @@
         <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="3">
+        <v>14</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>